<commit_message>
first Demo for UserEndpoint
write it in Jsonarray
</commit_message>
<xml_diff>
--- a/Arbeitszeit.xlsx
+++ b/Arbeitszeit.xlsx
@@ -160,16 +160,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.3765182186235"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
@@ -238,6 +238,11 @@
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>43403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>